<commit_message>
deleted old copies of data files created camera data folder drafted new scripts for analysing petal traits
</commit_message>
<xml_diff>
--- a/data/raw/plant/Petal_waterloss_time.xlsx
+++ b/data/raw/plant/Petal_waterloss_time.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretchen/GitHub/CApoppy/data/raw/plant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B9A533-411B-6946-BC65-9345A288280B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76C04EA-217F-DD49-B71A-8E509220235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="4640" windowWidth="28040" windowHeight="17440" xr2:uid="{16FA856C-A606-794D-9C8D-A4729CA9F9F1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Water loss recorded on 28 April 2025</t>
   </si>
@@ -99,7 +99,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -724,6 +724,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -731,7 +732,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1220,6 +1220,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1227,7 +1228,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2771,7 +2771,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2844,7 +2844,7 @@
         <v>9.1259999999999994E-2</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E22" si="0">D4/$D$2</f>
+        <f t="shared" ref="E4:E21" si="0">D4/$D$2</f>
         <v>0.99617945639122363</v>
       </c>
       <c r="F4" s="3">
@@ -3271,7 +3271,7 @@
         <v>0.91654929577464794</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ref="F24:F31" si="3">E23-E24</f>
+        <f t="shared" ref="F24:F29" si="3">E23-E24</f>
         <v>3.744131455399069E-2</v>
       </c>
     </row>
@@ -3298,6 +3298,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
       <c r="B26">
         <v>2</v>
       </c>
@@ -3317,6 +3320,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
       <c r="B27">
         <v>2</v>
       </c>
@@ -3336,6 +3342,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
       <c r="B28">
         <v>2</v>
       </c>
@@ -3355,6 +3364,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
       <c r="B29">
         <v>2</v>
       </c>
@@ -3374,6 +3386,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
       <c r="B30">
         <v>2</v>
       </c>
@@ -3390,6 +3405,9 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
       <c r="B31">
         <v>2</v>
       </c>

</xml_diff>